<commit_message>
Author : Ruchit Story Id: SSDMS 46 Description : Updated SCGJ Excel Sheets
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/SCGJ_Updated_Excel/Assessment_Agency.xlsx
+++ b/SSDMS_Requirements/SCGJ_Updated_Excel/Assessment_Agency.xlsx
@@ -91,7 +91,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -140,11 +140,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -157,7 +177,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,14 +479,14 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72" style="6" customWidth="1"/>
     <col min="4" max="15" width="8.88671875" style="5"/>
     <col min="16" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -479,13 +503,13 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -496,7 +520,7 @@
       <c r="B3" s="2">
         <v>123456</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author : Ruchit Jain Description : SCGJ Updated Excel Sheets
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/SCGJ_Updated_Excel/Assessment_Agency.xlsx
+++ b/SSDMS_Requirements/SCGJ_Updated_Excel/Assessment_Agency.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>agencyName</t>
   </si>
   <si>
     <t>Integer</t>
-  </si>
-  <si>
-    <t>CII(Confederation of Indian Industry)</t>
   </si>
   <si>
     <t>agencyId</t>
@@ -40,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +57,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,25 +96,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -128,19 +120,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -149,45 +128,49 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -476,56 +459,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="72" style="6" customWidth="1"/>
-    <col min="4" max="15" width="8.88671875" style="5"/>
-    <col min="16" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="17.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="85.6640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" s="7" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" s="7" customFormat="1">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2">
-        <v>123</v>
-      </c>
-      <c r="B3" s="2">
-        <v>123456</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>2</v>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="C97D" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C97D" sheet="1" objects="1" scenarios="1" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>